<commit_message>
feat: create classes from excel document
</commit_message>
<xml_diff>
--- a/uploads/horario.xlsx
+++ b/uploads/horario.xlsx
@@ -5864,15 +5864,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>70100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="70100" y="706320"/>
     <xdr:ext cx="8978900" cy="0"/>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5905,7 +5900,7 @@
       </xdr:spPr>
     </xdr:sp>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6250,15 +6245,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>70100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="70100" y="706320"/>
     <xdr:ext cx="8978900" cy="0"/>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6291,7 +6281,7 @@
       </xdr:spPr>
     </xdr:sp>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7300,6 +7290,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7321,7 +7312,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10287,6 +10277,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10329,7 +10320,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>